<commit_message>
basically final version of stimulus
</commit_message>
<xml_diff>
--- a/data/raw/my_risk (accessed 2017-12-06).xlsx
+++ b/data/raw/my_risk (accessed 2017-12-06).xlsx
@@ -1,15 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="29005"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelgiffin/Dropbox/RL/data/raw/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="21360" windowHeight="12580"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -862,8 +875,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -900,6 +913,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -946,12 +964,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -978,14 +996,15 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1012,6 +1031,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1187,14 +1207,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="19" max="19" width="20.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1283,7 +1308,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1345,7 +1370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1407,7 +1432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1469,7 +1494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:29">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1531,7 +1556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:29">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1587,7 +1612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1643,7 +1668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1699,7 +1724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:29">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1755,7 +1780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:29">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1817,7 +1842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:29">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1879,7 +1904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:29">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1935,7 +1960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:29">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1991,7 +2016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:29">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2032,7 +2057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:29">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
@@ -2094,7 +2119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:29">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -2156,7 +2181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:29">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1</v>
       </c>
@@ -2218,7 +2243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:29">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
@@ -2280,7 +2305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:29">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -2342,7 +2367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:29">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
@@ -2404,7 +2429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:29">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -2466,7 +2491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:29">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
@@ -2528,7 +2553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:29">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
@@ -2590,7 +2615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:29">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -2652,7 +2677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:29">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1</v>
       </c>
@@ -2714,7 +2739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:29">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1</v>
       </c>
@@ -2776,7 +2801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:29">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1</v>
       </c>
@@ -2838,7 +2863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:29">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1</v>
       </c>
@@ -2900,7 +2925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:29">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
@@ -2962,7 +2987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:29">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1</v>
       </c>
@@ -3024,7 +3049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:29">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1</v>
       </c>
@@ -3086,7 +3111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:29">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1</v>
       </c>
@@ -3148,7 +3173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:29">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1</v>
       </c>
@@ -3210,7 +3235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:29">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1</v>
       </c>
@@ -3272,7 +3297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:29">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1</v>
       </c>
@@ -3334,7 +3359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:29">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1</v>
       </c>
@@ -3396,7 +3421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:29">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1</v>
       </c>
@@ -3458,7 +3483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:29">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1</v>
       </c>
@@ -3520,7 +3545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:29">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1</v>
       </c>
@@ -3582,7 +3607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:29">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1</v>
       </c>
@@ -3623,7 +3648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:29">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1</v>
       </c>
@@ -3685,7 +3710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:29">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1</v>
       </c>
@@ -3747,7 +3772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:29">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>1</v>
       </c>
@@ -3809,7 +3834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:29">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1</v>
       </c>
@@ -3850,7 +3875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:29">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>1</v>
       </c>
@@ -3912,7 +3937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:29">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1</v>
       </c>
@@ -3974,7 +3999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:29">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1</v>
       </c>
@@ -4036,7 +4061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:29">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>1</v>
       </c>
@@ -4098,7 +4123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:29">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>1</v>
       </c>
@@ -4160,7 +4185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:29">
+    <row r="50" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>1</v>
       </c>
@@ -4222,7 +4247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:29">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>1</v>
       </c>
@@ -4284,7 +4309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:29">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>1</v>
       </c>
@@ -4346,7 +4371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:29">
+    <row r="53" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>1</v>
       </c>
@@ -4408,7 +4433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:29">
+    <row r="54" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>1</v>
       </c>
@@ -4470,7 +4495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:29">
+    <row r="55" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>1</v>
       </c>
@@ -4532,7 +4557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:29">
+    <row r="56" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>1</v>
       </c>
@@ -4594,7 +4619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:29">
+    <row r="57" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>1</v>
       </c>
@@ -4656,7 +4681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:29">
+    <row r="58" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>1</v>
       </c>
@@ -4718,7 +4743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:29">
+    <row r="59" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>1</v>
       </c>
@@ -4780,7 +4805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:29">
+    <row r="60" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>1</v>
       </c>
@@ -4842,7 +4867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:29">
+    <row r="61" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>1</v>
       </c>
@@ -4904,7 +4929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:29">
+    <row r="62" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>1</v>
       </c>
@@ -4966,7 +4991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:29">
+    <row r="63" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>1</v>
       </c>
@@ -5028,7 +5053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:29">
+    <row r="64" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>1</v>
       </c>
@@ -5090,7 +5115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:29">
+    <row r="65" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>1</v>
       </c>
@@ -5152,7 +5177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:29">
+    <row r="66" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>1</v>
       </c>

</xml_diff>